<commit_message>
CH 6 PA Upload
</commit_message>
<xml_diff>
--- a/Assignment Schedule.xlsx
+++ b/Assignment Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\programming\The-Principles-of-Deep-Learning1-Artificial-Neurons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36FE49E-78EB-44A0-8FE3-87F93BE07302}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC73F78-070D-41EF-8128-785D5C4DF0FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="119">
   <si>
     <t>Lecture</t>
   </si>
@@ -392,6 +392,30 @@
   </si>
   <si>
     <t>Q5-6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Polynomial Regression</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CH 6_01_01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CH 6_02_01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CH 6_03_01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CH 6_04_01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Q6-1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -443,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -451,6 +475,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -482,8 +510,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:F77" totalsRowShown="0">
-  <autoFilter ref="B3:F77" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:F83" totalsRowShown="0">
+  <autoFilter ref="B3:F83" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Chapter" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name=" "/>
@@ -792,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F77"/>
+  <dimension ref="B2:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J66" sqref="J66"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
@@ -1522,7 +1550,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D65" s="1" t="s">
         <v>89</v>
       </c>
@@ -1533,7 +1561,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="66" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D66" s="1" t="s">
         <v>90</v>
       </c>
@@ -1541,7 +1569,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="67" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D67" s="1" t="s">
         <v>91</v>
       </c>
@@ -1552,7 +1580,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="68" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D68" s="1" t="s">
         <v>92</v>
       </c>
@@ -1563,7 +1591,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D69" s="1" t="s">
         <v>93</v>
       </c>
@@ -1574,7 +1602,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D70" s="1" t="s">
         <v>94</v>
       </c>
@@ -1585,7 +1613,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="71" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D71" s="1" t="s">
         <v>95</v>
       </c>
@@ -1596,7 +1624,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D72" s="1" t="s">
         <v>96</v>
       </c>
@@ -1607,7 +1635,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D73" s="1" t="s">
         <v>97</v>
       </c>
@@ -1618,7 +1646,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="74" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D74" s="1" t="s">
         <v>98</v>
       </c>
@@ -1629,7 +1657,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D75" s="1" t="s">
         <v>99</v>
       </c>
@@ -1640,7 +1668,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D76" s="1" t="s">
         <v>100</v>
       </c>
@@ -1651,7 +1679,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="77" spans="4:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.45">
       <c r="D77" s="1" t="s">
         <v>101</v>
       </c>
@@ -1661,6 +1689,55 @@
       <c r="F77" s="1" t="s">
         <v>84</v>
       </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B78" s="1">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
+        <v>113</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D79" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D80" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="D81" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B82" s="3"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B83" s="3"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>